<commit_message>
إضافة إيفينت جديد في Card24 by admin at 2025-11-30 18:30:12
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,26 +561,66 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -598,19 +638,71 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,19 +720,71 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -658,19 +802,71 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -693,7 +889,11 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -714,17 +914,41 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -747,7 +971,11 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -758,19 +986,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -788,19 +1048,71 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -818,19 +1130,71 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -848,19 +1212,71 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -878,19 +1294,71 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -908,19 +1376,105 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>12\11\2024</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2251,66 +2805,18 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2343,51 +2849,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>15\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2405,66 +2879,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2482,11 +2908,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -2502,46 +2924,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>1\3\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2564,61 +2958,25 @@
           <t>591</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>19\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2641,36 +2999,20 @@
           <t>758</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -2681,21 +3023,9 @@
           <t>23\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2723,36 +3053,12 @@
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>30/11/2025</t>
@@ -2763,16 +3069,8 @@
           <t>م.محمد عبدالله ،خبير.ارول</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2795,11 +3093,7 @@
           <t>895</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -2810,46 +3104,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>13\10\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2867,66 +3133,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2944,66 +3162,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3021,66 +3191,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3098,66 +3220,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة إيفينت جديد في Card22 by admin at 2025-11-30 18:38:21
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -561,66 +561,26 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم التشغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -638,71 +598,19 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -720,71 +628,19 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -802,71 +658,19 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -889,11 +693,7 @@
           <t>632</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
@@ -914,41 +714,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>20\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -971,11 +747,7 @@
           <t>870</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -986,51 +758,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>6\10\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1048,71 +788,19 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1130,71 +818,19 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1212,71 +848,19 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1294,71 +878,19 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1376,71 +908,19 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -10442,7 +9922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10548,13 +10028,41 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>20\2\2024</t>
@@ -10565,7 +10073,11 @@
           <t xml:space="preserve">تم التشغيل </t>
         </is>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -10588,18 +10100,66 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10617,18 +10177,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10646,7 +10254,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10662,21 +10274,41 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>25\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O5" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -10704,25 +10336,61 @@
           <t>629</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>14\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10745,7 +10413,11 @@
           <t>800</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10756,18 +10428,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>1\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10785,18 +10485,66 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10814,18 +10562,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10843,18 +10639,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10872,18 +10716,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10901,18 +10793,99 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>12\11\2024</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card1 by admin at 2025-12-03 12:43:23
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -955,6 +955,128 @@
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>11\2\2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>وقت زيت</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>تم تغير زيت</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>950</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>1/12/2025</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>قطع سير كويلر 1270</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>تم تغير سير كويلر 1270</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>مصطفي</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>968</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم  سن دوغر وسلندر وفلاتس وعيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>خبير ارول</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5855,7 +5977,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5924,16 +6046,27 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>150</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -5944,16 +6077,23 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>151</v>
-      </c>
-      <c r="C3" t="n">
-        <v>300</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
@@ -5976,16 +6116,23 @@
           <t>6\8\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>301</v>
-      </c>
-      <c r="C4" t="n">
-        <v>450</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -5996,16 +6143,23 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>451</v>
-      </c>
-      <c r="C5" t="n">
-        <v>550</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
@@ -6036,19 +6190,28 @@
           <t>23\1\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>551</v>
-      </c>
-      <c r="C6" t="n">
-        <v>700</v>
-      </c>
-      <c r="D6" t="n">
-        <v>641</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -6066,19 +6229,28 @@
           <t>15\5\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>701</v>
-      </c>
-      <c r="C7" t="n">
-        <v>850</v>
-      </c>
-      <c r="D7" t="n">
-        <v>836</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
@@ -6100,16 +6272,23 @@
           <t>4\9\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="n">
-        <v>851</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -6120,16 +6299,23 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1150</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
@@ -6140,16 +6326,23 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1300</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
@@ -6160,16 +6353,23 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1301</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1450</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -6180,16 +6380,23 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1451</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1500</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
@@ -6200,6 +6407,38 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6513,7 +6752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7045,6 +7284,47 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2\12\2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>تم تغير</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>قطع سي1270</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>محمود</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8736,7 +9016,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8837,6 +9117,1371 @@
           <t>150</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1/2/2024</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم تشغيل الماكينه اول مره</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>زكريا</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>15\7\2024</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>11\8\2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4300 ساعه تشغيل</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>تم التشحيم شحم Ep3</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>29\9\2024</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>اعاده عيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>22\12\2024</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>صيانه نصف سنويه</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>تيم العمل</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>29\1\2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>5\4\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>5\7\2025</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>859</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>24\9\2025</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2\11\2025</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>قطع سير 1270</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>تغير سير 1270</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>تشحيم</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>333ساعه</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>card</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Tones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Tones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tones</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(x)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1.carding elemnt(o)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>licker_in carding element(o)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doffer carding element(o)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>cylinder(X)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>doffer(X)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(o)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -8845,27 +10490,23 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1/2/2024</t>
-        </is>
-      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>تم تشغيل الماكينه اول مره</t>
+          <t>تم الشتغيل</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>زكريا</t>
+          <t>A.Elshenawy</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -8878,11 +10519,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8900,7 +10537,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>15\7\2024</t>
+          <t>16\7\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -8910,62 +10547,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>450</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>11\8\2024</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4300 ساعه تشغيل</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>تم التشحيم شحم Ep3</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
+          <t>27\2\2025</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>550</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -8976,93 +10613,93 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>29\9\2024</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>زياره توكيل</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>اعاده عيار ماكينه</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>22\12\2024</t>
+          <t>7\4\2025</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>صيانه نصف سنويه</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>تيم العمل</t>
-        </is>
-      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>6\7\2025</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -9070,25 +10707,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9100,108 +10737,96 @@
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>29\1\2025</t>
+          <t>28\9\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>918</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>5\4\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
+          <t>1\11\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">تم سن فلاتس وعياره </t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>724</t>
-        </is>
-      </c>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>5\7\2025</t>
-        </is>
-      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -9209,40 +10834,28 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>859</t>
-        </is>
-      </c>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>24\9\2025</t>
-        </is>
-      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -9250,17 +10863,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1450</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -9279,17 +10892,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>1451</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -9308,20 +10921,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -9329,587 +10938,26 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>card</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min_Tones</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Tones</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tones</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(x)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>1.carding elemnt(o)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>licker_in carding element(o)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Doffer carding element(o)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cylinder(X)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>doffer(X)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(o)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم الشتغيل</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>A.Elshenawy</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>16\7\2024</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>27\2\2025</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>559</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>7\4\2025</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>6\7\2025</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>860</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>28\9\2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>م.محمد عبدالله</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>918</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>1\11\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">تم سن فلاتس وعياره </t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">م.محمد عبدالله </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10028,41 +11076,13 @@
           <t>.1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>20\2\2024</t>
@@ -10073,11 +11093,7 @@
           <t xml:space="preserve">تم التشغيل </t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -10100,66 +11116,18 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10177,66 +11145,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10254,11 +11174,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10274,41 +11190,21 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>25\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>م.صيام</t>
@@ -10336,61 +11232,25 @@
           <t>629</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>14\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10413,11 +11273,7 @@
           <t>800</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10428,46 +11284,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
           <t>1\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10485,66 +11313,18 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10562,66 +11342,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10639,66 +11371,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10716,66 +11400,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10793,66 +11429,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-12-03 13:23:13
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -9117,1371 +9117,6 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>1/2/2024</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>تم تشغيل الماكينه اول مره</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>زكريا</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>159</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>15\7\2024</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>11\8\2024</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>4300 ساعه تشغيل</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>تم التشحيم شحم Ep3</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>29\9\2024</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>زياره توكيل</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>اعاده عيار ماكينه</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>م.صيام</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>151</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>22\12\2024</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>صيانه نصف سنويه</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>تيم العمل</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>29\1\2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>551</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>565</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>5\4\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>701</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>724</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>5\7\2025</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>851</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>859</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>24\9\2025</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1001</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1151</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1301</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1450</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1451</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1500</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>2\2\2025</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>خلل ف عيار</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>تم اعاده عيار</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>م.عبدالله</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>990</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>2\11\2025</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>قطع سير 1270</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>تغير سير 1270</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>تشحيم</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>333ساعه</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>حسام</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>card</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Min_Tones</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Tones</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Tones</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(x)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>1.carding elemnt(o)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>licker_in carding element(o)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Doffer carding element(o)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>cylinder(X)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>doffer(X)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Revolving flats(o)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Correction</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Serviced by</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -10490,23 +9125,27 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1/2/2024</t>
+        </is>
+      </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>تم الشتغيل</t>
+          <t>تم تشغيل الماكينه اول مره</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
-          <t>A.Elshenawy</t>
+          <t>زكريا</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -10519,7 +9158,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10537,7 +9180,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>16\7\2024</t>
+          <t>15\7\2024</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -10547,62 +9190,62 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>301</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>27\2\2025</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+          <t>11\8\2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>4300 ساعه تشغيل</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>تم التشحيم شحم Ep3</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>451</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>550</t>
+          <t>300</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -10613,93 +9256,93 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>29\9\2024</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>زياره توكيل</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>اعاده عيار ماكينه</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>م.صيام</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>551</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>700</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>559</t>
-        </is>
-      </c>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>7\4\2025</t>
+          <t>22\12\2024</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>صيانه نصف سنويه</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>تيم العمل</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>301</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>727</t>
-        </is>
-      </c>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>6\7\2025</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -10707,25 +9350,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>451</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>860</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10737,96 +9380,108 @@
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>28\9\2025</t>
+          <t>29\1\2025</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>م.محمد عبدالله</t>
-        </is>
-      </c>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>851</t>
+          <t>551</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>700</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>918</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>✔</t>
-        </is>
-      </c>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1\11\2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">تم سن فلاتس وعياره </t>
-        </is>
-      </c>
+          <t>5\4\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">م.محمد عبدالله </t>
-        </is>
-      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1001</t>
+          <t>701</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1150</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>724</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>5\7\2025</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
@@ -10834,28 +9489,40 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1151</t>
+          <t>851</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1300</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>859</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>24\9\2025</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
@@ -10863,17 +9530,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1301</t>
+          <t>1001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1450</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -10892,17 +9559,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1451</t>
+          <t>1151</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1300</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -10921,16 +9588,20 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -10938,6 +9609,1235 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2\2\2025</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>خلل ف عيار</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>تم اعاده عيار</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2\11\2025</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>قطع سير 1270</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>تغير سير 1270</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>تشحيم</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>333ساعه</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>حسام</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>card</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Min_Tones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Max_Tones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tones</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(x)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1.carding elemnt(o)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>licker_in carding element(o)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Doffer carding element(o)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>cylinder(X)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>doffer(X)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Revolving flats(o)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Serviced by</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>تم الشتغيل</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>A.Elshenawy</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>16\7\2024</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>27\2\2025</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>550</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>551</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>559</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>7\4\2025</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>6\7\2025</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>860</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>28\9\2025</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>م.محمد عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>918</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>✔</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>1\11\2025</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">تم سن فلاتس وعياره </t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">م.محمد عبدالله </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1150</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1450</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1451</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>2\2\2025</t>
@@ -10956,6 +10856,39 @@
       <c r="O14" t="inlineStr">
         <is>
           <t>م.عبدالله</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>ححح</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-12-03 13:23:23
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -9773,7 +9773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10865,28 +10865,105 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>1111</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O15" t="inlineStr">
+        <is>
+          <t>ححح</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
         <is>
           <t>ححح</t>
         </is>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card2 by admin at 2025-12-03 13:23:26
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -9773,7 +9773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10942,28 +10942,105 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
           <t>1111</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O16" t="inlineStr">
+        <is>
+          <t>ححح</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>1111</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
         <is>
           <t>ححح</t>
         </is>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card8 by admin at 2025-12-03 14:19:29
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -4470,7 +4470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4571,18 +4571,66 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4600,7 +4648,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4611,19 +4663,51 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>1\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4641,18 +4725,66 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4670,7 +4802,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4686,22 +4822,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>20\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4724,25 +4884,61 @@
           <t>573</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>12\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4765,16 +4961,36 @@
           <t>742</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4785,9 +5001,21 @@
           <t>17\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -4815,19 +5043,51 @@
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
           <t>25/11/2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله ،ف.محمود ايهاب</t>
@@ -4855,7 +5115,11 @@
           <t>873</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4866,18 +5130,46 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr">
         <is>
           <t>4\10\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4895,18 +5187,66 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -4924,18 +5264,66 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -4953,18 +5341,66 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4982,18 +5418,103 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>تم تغير السير</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>قطع سير</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>درش</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9874,61 +10395,21 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>تم الشتغيل</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>A.Elshenawy</t>
@@ -9951,11 +10432,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -9966,51 +10443,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>16\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10028,11 +10473,7 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10048,46 +10489,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>27\2\2025</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10105,66 +10518,18 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10187,61 +10552,25 @@
           <t>559</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>7\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10264,36 +10593,16 @@
           <t>727</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10304,21 +10613,9 @@
           <t>6\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10341,11 +10638,7 @@
           <t>860</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>✔</t>
@@ -10356,41 +10649,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>28\9\2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله</t>
@@ -10423,36 +10692,12 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>1\11\2025</t>
@@ -10463,11 +10708,7 @@
           <t xml:space="preserve">تم سن فلاتس وعياره </t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t xml:space="preserve">م.محمد عبدالله </t>
@@ -10490,66 +10731,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -10567,66 +10760,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -10644,66 +10789,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -10721,66 +10818,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -10788,56 +10837,20 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
           <t>2\2\2025</t>
@@ -10865,71 +10878,27 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
           <t>1111</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>ححح</t>
@@ -10942,71 +10911,27 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
           <t>1111</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>ححح</t>

</xml_diff>

<commit_message>
إضافة حدث جديد في Card23 by admin at 2025-12-06 12:53:28
</commit_message>
<xml_diff>
--- a/elquds2.xlsx
+++ b/elquds2.xlsx
@@ -4571,66 +4571,18 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4648,11 +4600,7 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4663,51 +4611,19 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>1\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4725,66 +4641,18 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4802,11 +4670,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -4822,46 +4686,22 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>20\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4884,61 +4724,25 @@
           <t>573</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>12\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4961,36 +4765,16 @@
           <t>742</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5001,21 +4785,9 @@
           <t>17\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5043,51 +4815,19 @@
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>25/11/2025</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>م.محمد عبدالله ،ف.محمود ايهاب</t>
@@ -5115,11 +4855,7 @@
           <t>873</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -5130,46 +4866,18 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>4\10\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -5187,66 +4895,18 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -5264,66 +4924,18 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -5341,66 +4953,18 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -5418,66 +4982,18 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -6498,7 +6014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6572,6 +6088,16 @@
           <t>Servised by</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6589,16 +6115,58 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -6616,7 +6184,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6627,17 +6199,43 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>6\8\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -6655,16 +6253,58 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -6682,7 +6322,11 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6698,20 +6342,38 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6734,23 +6396,53 @@
           <t>641</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>15\5\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6773,7 +6465,11 @@
           <t>836</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -6784,16 +6480,38 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>4\9\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6811,16 +6529,58 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6838,16 +6598,58 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -6865,16 +6667,58 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -6892,16 +6736,58 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -6919,16 +6805,58 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -6936,20 +6864,56 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr">
         <is>
           <t>2\2\2025</t>
@@ -6958,6 +6922,45 @@
       <c r="M13" t="inlineStr">
         <is>
           <t>م.عبدالله</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>6/12/2025</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>م محمد عبدالله وتيم الكرد</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>خلل ف جوده</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>تغير فلاتس متحركه واول جريده240 وسن دوفر وسلندر 6شوط</t>
         </is>
       </c>
     </row>

</xml_diff>